<commit_message>
chore!: remove input value IOP_fraction from conductor_operation input files.
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_1_operation.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_1_operation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/Description_of_Components/input_file_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/input_files/input_file_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{6F6F60DD-9A76-4126-9A28-D0FBB56FD81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA1F6644-7BFB-44AA-81D5-D419D8C9AEB5}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{6F6F60DD-9A76-4126-9A28-D0FBB56FD81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BCFB2D1-34DD-4FA5-82B5-2D6FFA26F2FC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAN" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="106">
   <si>
     <t>IBIFUN</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Q0</t>
   </si>
   <si>
-    <t>IOP0_FRACTION</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
@@ -170,9 +167,6 @@
   </si>
   <si>
     <t>element of the type "SC+Cu strands"</t>
-  </si>
-  <si>
-    <t>fraction of IOP0 tranported at time = 0 by the strand</t>
   </si>
   <si>
     <t>flag to define the magnetic field gradient along the strand: 0 = no gradient, -1 = read from file "alphab.dat"</t>
@@ -985,17 +979,17 @@
       <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.140625" style="4" customWidth="1"/>
-    <col min="5" max="6" width="17.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="5"/>
+    <col min="1" max="1" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.1796875" style="4" customWidth="1"/>
+    <col min="5" max="6" width="17.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="str">
         <f>[1]CHAN!$A$1</f>
         <v>CHAN</v>
@@ -1006,7 +1000,7 @@
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E1" s="13">
         <f>[2]CHAN!E$1</f>
@@ -1017,12 +1011,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="6"/>
       <c r="D2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="13">
         <f>IF(E$1 &gt; 0,1,0)</f>
@@ -1033,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="str">
         <f>[1]CHAN!A$3</f>
         <v>Variable name</v>
@@ -1059,18 +1053,18 @@
         <v>CHAN_2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="3">
         <v>2</v>
@@ -1079,18 +1073,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E5" s="3">
         <v>4.5</v>
@@ -1099,18 +1093,18 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E6" s="3">
         <v>4.5</v>
@@ -1119,18 +1113,18 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E7" s="3">
         <v>4.5</v>
@@ -1139,18 +1133,18 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E8" s="9">
         <v>600000</v>
@@ -1159,18 +1153,18 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E9" s="26">
         <v>590000</v>
@@ -1179,18 +1173,18 @@
         <v>590000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E10" s="9">
         <f>600000</f>
@@ -1201,18 +1195,18 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E11" s="3">
         <v>8.3999999999999995E-3</v>
@@ -1221,24 +1215,24 @@
         <v>1.248E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1250,26 +1244,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD9"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.42578125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="5"/>
+    <col min="1" max="1" width="27.7265625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.453125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="str">
         <f>[1]STR_MIX!$A$1</f>
         <v>STR_MIX</v>
@@ -1280,26 +1274,26 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="13">
         <f>[2]STR_MIX!E$1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="18"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="13">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -1321,63 +1315,63 @@
         <v>STR_MIX_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>27</v>
+        <v>82</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>75</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>84</v>
       </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="29" t="s">
+        <v>97</v>
+      </c>
       <c r="B5" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="E5" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>26</v>
+      <c r="B6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="29" t="s">
         <v>101</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>26</v>
@@ -1389,92 +1383,92 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="29" t="s">
         <v>103</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E8" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>27</v>
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>25</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="E9" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="D10" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>20</v>
       </c>
@@ -1482,33 +1476,31 @@
         <v>1</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E13" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>22</v>
       </c>
@@ -1516,329 +1508,314 @@
         <v>1</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="D18" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="E21" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="20" t="s">
+      <c r="E22" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>35</v>
-      </c>
       <c r="B23" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="D23" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E23" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E23" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>77</v>
+        <v>6</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="E24" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B26" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" s="24">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
         <v>38</v>
       </c>
       <c r="B28" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A30" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E28" s="24">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="24">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+      <c r="B30" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="D30" s="20" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E30" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C31" s="24" t="s">
         <v>26</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E31" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E32" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="E33" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B34" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E34" s="24" t="b">
+      <c r="E33" s="24" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1851,27 +1828,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04312A78-FBC2-476F-A763-194D3CD2A19F}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D10" sqref="D10"/>
       <selection pane="topRight" activeCell="D10" sqref="D10"/>
       <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.42578125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="5"/>
+    <col min="1" max="1" width="27.7265625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.453125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="str">
         <f>[1]STR_SC!$A$1</f>
         <v>STR_SC</v>
@@ -1882,26 +1859,26 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E1" s="13">
         <f>[2]STR_STAB!E$1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="18"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="13">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -1923,63 +1900,63 @@
         <v>STR_SC_0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>27</v>
+        <v>82</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>75</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>84</v>
       </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="29" t="s">
+        <v>97</v>
+      </c>
       <c r="B5" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="E5" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>26</v>
+      <c r="B6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="29" t="s">
         <v>101</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>26</v>
@@ -1991,92 +1968,92 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="29" t="s">
         <v>103</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E8" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>27</v>
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>25</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="E9" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="D10" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>20</v>
       </c>
@@ -2084,33 +2061,31 @@
         <v>1</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E13" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>22</v>
       </c>
@@ -2118,329 +2093,314 @@
         <v>1</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="D18" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="E21" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="20" t="s">
+      <c r="E22" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>35</v>
-      </c>
       <c r="B23" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="D23" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E23" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E23" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>77</v>
+        <v>6</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="E24" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B26" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
         <v>38</v>
       </c>
       <c r="B28" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A30" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E28" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+      <c r="B30" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="D30" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E30" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="E30" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C31" s="24" t="s">
         <v>26</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E31" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E32" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B34" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E34" s="24" t="b">
+      <c r="E33" s="24" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2452,27 +2412,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791C09E2-9ECD-4150-8BC7-6143A0B898FB}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D22" sqref="D22"/>
       <selection pane="topRight" activeCell="D22" sqref="D22"/>
       <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
-      <selection pane="bottomRight" sqref="A1:A1048576"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="5"/>
+    <col min="1" max="1" width="27.7265625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.453125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="str">
         <f>[1]STR_STAB!$A$1</f>
         <v>STR_STAB</v>
@@ -2483,26 +2443,26 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E1" s="13">
         <f>[2]STR_SC!E$1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="18"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" s="13">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -2524,63 +2484,63 @@
         <v>STR_STAB_0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>27</v>
+        <v>82</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>75</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>84</v>
       </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="29" t="s">
+        <v>97</v>
+      </c>
       <c r="B5" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="E5" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>26</v>
+      <c r="B6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="29" t="s">
         <v>101</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>26</v>
@@ -2592,92 +2552,92 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="29" t="s">
         <v>103</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E8" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>27</v>
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>25</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="E9" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="D10" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>20</v>
       </c>
@@ -2685,33 +2645,31 @@
         <v>1</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E13" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>22</v>
       </c>
@@ -2719,261 +2677,246 @@
         <v>1</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="E19" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="D20" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E20" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E20" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="E21" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>47</v>
+        <v>26</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>46</v>
       </c>
       <c r="E22" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B23" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>48</v>
+        <v>26</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="E23" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="B24" s="24" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="E24" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A27" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E26" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+      <c r="B27" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>52</v>
+      <c r="D27" s="20" t="s">
+        <v>68</v>
       </c>
       <c r="E27" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C28" s="24" t="s">
         <v>26</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E28" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E29" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="E30" s="27">
         <v>0</v>
       </c>
     </row>
@@ -2986,27 +2929,27 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D22" sqref="D22"/>
       <selection pane="topRight" activeCell="D22" sqref="D22"/>
       <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD25"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="5"/>
+    <col min="1" max="1" width="14.453125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.453125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="str">
         <f>[1]Z_JACKET!$A$1</f>
         <v>Z_JACKET</v>
@@ -3017,26 +2960,26 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E1" s="13">
         <f>[2]Z_JACKET!E$1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="18"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="13">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -3058,92 +3001,92 @@
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>27</v>
+        <v>82</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>75</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>0</v>
-      </c>
       <c r="B6" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="D6" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>20</v>
       </c>
@@ -3151,33 +3094,31 @@
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E9" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
         <v>22</v>
       </c>
@@ -3185,244 +3126,229 @@
         <v>1</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="E15" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E16" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E16" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B19" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E19" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E20" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A22" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>39</v>
-      </c>
       <c r="B22" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>51</v>
+        <v>27</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>71</v>
       </c>
       <c r="E22" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C23" s="24" t="s">
         <v>26</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E23" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E24" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="E25" s="24">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: new input value in sheets (except CHAN)
Added input value flag IOP_MODE in sheet STACK, STR_MIX, STR_STAB and Z_JACKET.
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_1_operation.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_1_operation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/input_files/input_file_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{6F6F60DD-9A76-4126-9A28-D0FBB56FD81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35255F5B-DDD7-41AF-81EC-29A72829D624}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEAC1B7-B9DC-461B-8F51-72ED101B6B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3585" yWindow="3585" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAN" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="108">
   <si>
     <t>IBIFUN</t>
   </si>
@@ -359,6 +359,12 @@
   </si>
   <si>
     <t>Outlet STACK temperature</t>
+  </si>
+  <si>
+    <t>IOP_MODE</t>
+  </si>
+  <si>
+    <t>Flag to define how the current is defined: 0 = constant; -1 = read from file (only if I0_OP_MODE = -1 in sheet CONDUCTOR_input of input file conductor_definition.xlsx; none = no current for the object (typically used for the jacket components since at the time being it is assumed that they do not carry a current).</t>
   </si>
 </sst>
 </file>
@@ -427,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -475,18 +481,18 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -513,15 +519,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -981,17 +979,17 @@
       <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.1796875" style="4" customWidth="1"/>
-    <col min="5" max="6" width="17.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.81640625" style="5"/>
+    <col min="1" max="1" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.140625" style="4" customWidth="1"/>
+    <col min="5" max="6" width="17.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="str">
         <f>[1]CHAN!$A$1</f>
         <v>CHAN</v>
@@ -1013,7 +1011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="6"/>
@@ -1029,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="str">
         <f>[1]CHAN!A$3</f>
         <v>Variable name</v>
@@ -1055,7 +1053,7 @@
         <v>CHAN_2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>9</v>
       </c>
@@ -1071,11 +1069,11 @@
       <c r="E4" s="3">
         <v>2</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="25">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1091,11 +1089,11 @@
       <c r="E5" s="3">
         <v>4.5</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="25">
         <v>4.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -1111,11 +1109,11 @@
       <c r="E6" s="3">
         <v>4.5</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="25">
         <v>4.5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -1131,11 +1129,11 @@
       <c r="E7" s="3">
         <v>4.5</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="25">
         <v>4.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -1151,11 +1149,11 @@
       <c r="E8" s="9">
         <v>600000</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="26">
         <v>600000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -1168,14 +1166,14 @@
       <c r="D9" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="9">
         <v>590000</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="26">
         <v>590000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -1192,12 +1190,12 @@
         <f>600000</f>
         <v>600000</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="26">
         <f>600000</f>
         <v>600000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
@@ -1213,27 +1211,27 @@
       <c r="E11" s="3">
         <v>8.3999999999999995E-3</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="25">
         <v>1.248E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="24" t="s">
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="3" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1249,24 +1247,24 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D10" sqref="D10"/>
       <selection pane="topRight" activeCell="D10" sqref="D10"/>
       <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
-      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7265625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.453125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.81640625" style="5"/>
+    <col min="1" max="1" width="27.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.42578125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="str">
         <f>[1]STACK!$A$1</f>
         <v>STACK</v>
@@ -1284,7 +1282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1296,7 +1294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -1318,42 +1316,42 @@
         <v>STACK_0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>72</v>
+        <v>106</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="24" t="s">
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="29" t="s">
+      <c r="E5" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
         <v>96</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -1365,12 +1363,12 @@
       <c r="D6" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="E6" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="29" t="s">
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
         <v>98</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -1382,12 +1380,12 @@
       <c r="D7" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="29" t="s">
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
         <v>100</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1399,66 +1397,66 @@
       <c r="D8" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="24" t="s">
+      <c r="B9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E9" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="24" t="s">
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="24" t="s">
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E11" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -1467,15 +1465,15 @@
       <c r="D12" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -1484,11 +1482,11 @@
       <c r="D13" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>21</v>
       </c>
@@ -1503,7 +1501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>22</v>
       </c>
@@ -1518,7 +1516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>23</v>
       </c>
@@ -1533,79 +1531,79 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="24" t="s">
+      <c r="B17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="24" t="s">
+      <c r="B18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="24" t="s">
+      <c r="B19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E19" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="24" t="s">
+      <c r="B20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D20" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="7" t="s">
@@ -1618,45 +1616,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="24" t="s">
+      <c r="B22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D22" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="E22" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B23" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="24" t="s">
+      <c r="B23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D23" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1665,15 +1663,15 @@
       <c r="D24" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="E24" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E24" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="7" t="s">
@@ -1682,15 +1680,15 @@
       <c r="D25" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E25" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -1699,15 +1697,15 @@
       <c r="D26" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E26" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="7" t="s">
@@ -1716,15 +1714,15 @@
       <c r="D27" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="E27" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E27" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -1733,15 +1731,15 @@
       <c r="D28" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E28" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C29" s="7" t="s">
@@ -1750,75 +1748,75 @@
       <c r="D29" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="E29" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="24" t="s">
+      <c r="B30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="E30" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D31" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="E31" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D32" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="E32" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="24" t="s">
+      <c r="B33" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>77</v>
       </c>
       <c r="D33" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="E33" s="24" t="b">
+      <c r="E33" s="3" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1830,7 +1828,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
@@ -1839,17 +1837,17 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7265625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.453125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.81640625" style="5"/>
+    <col min="1" max="1" width="27.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.42578125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="str">
         <f>[1]STR_MIX!$A$1</f>
         <v>STR_MIX</v>
@@ -1867,7 +1865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1879,7 +1877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -1901,194 +1899,196 @@
         <v>STR_MIX_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D5" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E5" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="29" t="s">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="24" t="s">
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D6" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="29" t="s">
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="B7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D7" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="E6" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="29" t="s">
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="20" t="s">
+      <c r="C8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="29" t="s">
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B9" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="20" t="s">
+      <c r="C9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="24" t="s">
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D10" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+      <c r="E10" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="24" t="s">
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D11" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E11" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="24" t="s">
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D12" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
+      <c r="E12" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="20" t="s">
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="20" t="s">
+      <c r="B14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="19" t="s">
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
         <v>21</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="19" t="s">
-        <v>22</v>
       </c>
       <c r="B15" s="23" t="s">
         <v>1</v>
@@ -2101,12 +2101,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>26</v>
@@ -2116,292 +2116,307 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="15" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="24" t="s">
+      <c r="B18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D18" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="15" t="s">
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="24" t="s">
+      <c r="B19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D19" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E19" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="15" t="s">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="24" t="s">
+      <c r="B20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D20" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="15" t="s">
+      <c r="E20" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="24" t="s">
+      <c r="B21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D21" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E21" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="15" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="20" t="s">
+      <c r="B22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="15" t="s">
+      <c r="E22" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="24" t="s">
+      <c r="B23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D23" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="E22" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="15" t="s">
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B23" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="24" t="s">
+      <c r="B24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D24" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E24" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="15" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="20" t="s">
+      <c r="C25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="E24" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="15" t="s">
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="20" t="s">
+      <c r="C26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="24">
+      <c r="E26" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="15" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B27" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="20" t="s">
+      <c r="C27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="24">
+      <c r="E27" s="3">
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="15" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="20" t="s">
+      <c r="C28" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="E27" s="24">
+      <c r="E28" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="15" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="20" t="s">
+      <c r="C29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="24">
+      <c r="E29" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="15" t="s">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="20" t="s">
+      <c r="B30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A30" s="15" t="s">
+      <c r="E30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="24" t="s">
+      <c r="B31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D31" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E30" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="15" t="s">
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B32" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D31" s="20" t="s">
+      <c r="C32" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="15" t="s">
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B33" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="20" t="s">
+      <c r="C33" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="15" t="s">
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="24" t="s">
+      <c r="B34" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D33" s="20" t="s">
+      <c r="D34" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="E33" s="24" t="b">
+      <c r="E34" s="3" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2424,17 +2439,17 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7265625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.453125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.81640625" style="5"/>
+    <col min="1" max="1" width="27.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="str">
         <f>[1]STR_STAB!$A$1</f>
         <v>STR_STAB</v>
@@ -2452,7 +2467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2464,7 +2479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -2486,42 +2501,42 @@
         <v>STR_STAB_0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>72</v>
+        <v>106</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="24" t="s">
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="29" t="s">
+      <c r="E5" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
         <v>96</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -2533,12 +2548,12 @@
       <c r="D6" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="E6" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="29" t="s">
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
         <v>98</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -2550,12 +2565,12 @@
       <c r="D7" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="29" t="s">
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
         <v>100</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -2567,66 +2582,66 @@
       <c r="D8" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="24" t="s">
+      <c r="B9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E9" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="24" t="s">
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="24" t="s">
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E11" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -2635,15 +2650,15 @@
       <c r="D12" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -2652,11 +2667,11 @@
       <c r="D13" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>21</v>
       </c>
@@ -2671,7 +2686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>22</v>
       </c>
@@ -2686,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>23</v>
       </c>
@@ -2701,79 +2716,79 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="24" t="s">
+      <c r="B17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="24" t="s">
+      <c r="B18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="24" t="s">
+      <c r="B19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="E19" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="24" t="s">
+      <c r="B20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D20" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="7" t="s">
@@ -2786,11 +2801,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="7" t="s">
@@ -2803,11 +2818,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="7" t="s">
@@ -2820,11 +2835,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -2833,15 +2848,15 @@
       <c r="D24" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E24" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="7" t="s">
@@ -2850,15 +2865,15 @@
       <c r="D25" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E25" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -2867,58 +2882,58 @@
       <c r="D26" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="E26" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="24" t="s">
+      <c r="B27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D27" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E27" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E27" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D28" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E28" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D29" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E29" s="25">
         <v>0</v>
       </c>
     </row>
@@ -2941,17 +2956,17 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.453125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.453125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.81640625" style="5"/>
+    <col min="1" max="1" width="14.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="str">
         <f>[1]Z_JACKET!$A$1</f>
         <v>Z_JACKET</v>
@@ -2969,7 +2984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2981,7 +2996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -3003,79 +3018,79 @@
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>72</v>
+        <v>106</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="24" t="s">
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E5" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="24" t="s">
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="24" t="s">
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E7" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -3084,15 +3099,15 @@
       <c r="D8" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -3101,11 +3116,11 @@
       <c r="D9" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E9" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>21</v>
       </c>
@@ -3120,7 +3135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>22</v>
       </c>
@@ -3135,7 +3150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>23</v>
       </c>
@@ -3150,79 +3165,79 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="24" t="s">
+      <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="24" t="s">
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="24" t="s">
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="E15" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="24" t="s">
+      <c r="B16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -3231,15 +3246,15 @@
       <c r="D17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -3248,15 +3263,15 @@
       <c r="D18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -3265,15 +3280,15 @@
       <c r="D19" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -3282,15 +3297,15 @@
       <c r="D20" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="7" t="s">
@@ -3299,58 +3314,58 @@
       <c r="D21" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="24" t="s">
+      <c r="B22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D22" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D23" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D24" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="24">
+      <c r="E24" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: new input variable in sheet CHAN template_conductor_1_operation.xlsx
Added new input variable MDTOUT in sheet CHAN of input file template_conductor_1_operation.xlsx

modified:   input_files/input_file_template/template_conductor_1_operation.xlsx
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_1_operation.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_1_operation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEAC1B7-B9DC-461B-8F51-72ED101B6B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E37271-24C5-4A43-931C-55DE61207307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="3585" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAN" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="110">
   <si>
     <t>IBIFUN</t>
   </si>
@@ -365,6 +365,12 @@
   </si>
   <si>
     <t>Flag to define how the current is defined: 0 = constant; -1 = read from file (only if I0_OP_MODE = -1 in sheet CONDUCTOR_input of input file conductor_definition.xlsx; none = no current for the object (typically used for the jacket components since at the time being it is assumed that they do not carry a current).</t>
+  </si>
+  <si>
+    <t>MDTOUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">outlet mass flow rate </t>
   </si>
 </sst>
 </file>
@@ -970,13 +976,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,23 +1221,43 @@
         <v>1.248E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D13" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1246,7 +1272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04312A78-FBC2-476F-A763-194D3CD2A19F}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D10" sqref="D10"/>
       <selection pane="topRight" activeCell="D10" sqref="D10"/>

</xml_diff>

<commit_message>
chore: add input variable in STR_STAB abd Z_JACKET in template_conductor_1_operation.xlsx
Added missing input variable IOP_INTERPOLATOR in sheets STR_STAB and Z_JACKET of input file template_conductor_1_operation.xlsx.
Notes are updated accordingly.

modified:   input_files/input_file_template/template_conductor_1_operation.xlsx
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_1_operation.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_1_operation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E37271-24C5-4A43-931C-55DE61207307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA84DA6C-0BF0-4535-B63D-08807F417C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAN" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="111">
   <si>
     <t>IBIFUN</t>
   </si>
@@ -371,6 +371,9 @@
   </si>
   <si>
     <t xml:space="preserve">outlet mass flow rate </t>
+  </si>
+  <si>
+    <t>Flag to specify the kind of interpolator for the operating current data, if IOP_MODE = -1. Possible values: linear = liear interpolation; cubic = use spline function of third order.</t>
   </si>
 </sst>
 </file>
@@ -978,7 +981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -1860,7 +1863,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1953,7 +1956,7 @@
         <v>72</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>81</v>
@@ -2455,14 +2458,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791C09E2-9ECD-4150-8BC7-6143A0B898FB}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D22" sqref="D22"/>
       <selection pane="topRight" activeCell="D22" sqref="D22"/>
       <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2545,51 +2548,51 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D6" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="B7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D7" s="20" t="s">
         <v>97</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>99</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
@@ -2597,58 +2600,58 @@
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B9" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="20" t="s">
+      <c r="C9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D10" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="E10" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>83</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>71</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>27</v>
@@ -2657,32 +2660,32 @@
         <v>72</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="24" t="s">
         <v>1</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>1</v>
@@ -2691,30 +2694,32 @@
         <v>26</v>
       </c>
       <c r="D13" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="23">
+      <c r="E14" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="23" t="s">
         <v>1</v>
@@ -2729,10 +2734,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>26</v>
@@ -2742,94 +2747,92 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D18" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="B19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D19" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="B20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D20" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="E19" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="B21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D21" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="8">
-        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>6</v>
@@ -2837,8 +2840,8 @@
       <c r="C22" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="20" t="s">
-        <v>46</v>
+      <c r="D22" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="E22" s="8">
         <v>0</v>
@@ -2846,16 +2849,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>47</v>
+      <c r="D23" s="20" t="s">
+        <v>46</v>
       </c>
       <c r="E23" s="8">
         <v>0</v>
@@ -2863,24 +2866,24 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="25">
+        <v>47</v>
+      </c>
+      <c r="E24" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>8</v>
@@ -2889,58 +2892,58 @@
         <v>26</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
+      <c r="E26" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="4" t="s">
+      <c r="B27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+      <c r="E27" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="B28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D28" s="20" t="s">
         <v>65</v>
-      </c>
-      <c r="E27" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>66</v>
       </c>
       <c r="E28" s="25">
         <v>0</v>
@@ -2948,7 +2951,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>14</v>
@@ -2957,9 +2960,26 @@
         <v>26</v>
       </c>
       <c r="D29" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E30" s="25">
         <v>0</v>
       </c>
     </row>
@@ -2972,14 +2992,14 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D22" sqref="D22"/>
       <selection pane="topRight" activeCell="D22" sqref="D22"/>
       <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
+      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3061,43 +3081,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D6" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>83</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>71</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>27</v>
@@ -3106,32 +3126,32 @@
         <v>72</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="24" t="s">
         <v>1</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>1</v>
@@ -3140,30 +3160,32 @@
         <v>26</v>
       </c>
       <c r="D9" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="23">
+      <c r="E10" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>1</v>
@@ -3178,10 +3200,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>26</v>
@@ -3191,94 +3213,92 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D14" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D15" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D16" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="E15" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="B17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D17" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>6</v>
@@ -3287,7 +3307,7 @@
         <v>26</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E18" s="3">
         <v>0</v>
@@ -3295,16 +3315,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E19" s="3">
         <v>0</v>
@@ -3312,16 +3332,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E20" s="3">
         <v>0</v>
@@ -3329,7 +3349,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>8</v>
@@ -3338,41 +3358,41 @@
         <v>26</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="B23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D23" s="20" t="s">
         <v>68</v>
-      </c>
-      <c r="E22" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>69</v>
       </c>
       <c r="E23" s="3">
         <v>0</v>
@@ -3380,7 +3400,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>14</v>
@@ -3389,9 +3409,26 @@
         <v>26</v>
       </c>
       <c r="D24" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E25" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
doc: improve documentation of flag INTIAL
Improved documentation related to flag INTIAL in input file template_conductor_1_operation.xlsx

modified:   input_files/input_file_template/template_conductor_1_operation.xlsx
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_1_operation.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_1_operation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA84DA6C-0BF0-4535-B63D-08807F417C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3EFA9B-407E-4A05-A0CC-8AD9A4A1EEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAN" sheetId="4" r:id="rId1"/>
@@ -163,9 +163,6 @@
     <t>element of the type fluid</t>
   </si>
   <si>
-    <t>flag to define the hydraulic boundary conditions (&gt;0 value from below, &lt;0 valure from input file: press.dat, temp.dat, mdot.dat)</t>
-  </si>
-  <si>
     <t>element of the type "SC+Cu strands"</t>
   </si>
   <si>
@@ -374,6 +371,9 @@
   </si>
   <si>
     <t>Flag to specify the kind of interpolator for the operating current data, if IOP_MODE = -1. Possible values: linear = liear interpolation; cubic = use spline function of third order.</t>
+  </si>
+  <si>
+    <t>flag to define initialization and the hydraulic boundary conditions (&gt;0 value from below, &lt;0 valure from input file: press.dat, temp.dat, mdot.dat). 1 = inlet and outlet pressure, inlet (outlet) temperaure; 2 = inlet pressure and temperature, outlet mass flow rate; 3 = inlet mass flow rate and temperature, outlet pressure.</t>
   </si>
 </sst>
 </file>
@@ -981,11 +981,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,7 +1062,7 @@
         <v>CHAN_2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>9</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="E4" s="3">
         <v>2</v>
@@ -1093,7 +1093,7 @@
         <v>26</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" s="3">
         <v>4.5</v>
@@ -1113,7 +1113,7 @@
         <v>26</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" s="3">
         <v>4.5</v>
@@ -1133,7 +1133,7 @@
         <v>26</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="3">
         <v>4.5</v>
@@ -1153,7 +1153,7 @@
         <v>26</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="9">
         <v>600000</v>
@@ -1173,7 +1173,7 @@
         <v>26</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" s="9">
         <v>590000</v>
@@ -1193,7 +1193,7 @@
         <v>26</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" s="9">
         <f>600000</f>
@@ -1215,7 +1215,7 @@
         <v>26</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" s="3">
         <v>8.3999999999999995E-3</v>
@@ -1226,7 +1226,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>17</v>
@@ -1235,7 +1235,7 @@
         <v>26</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E12" s="3">
         <v>0</v>
@@ -1246,22 +1246,22 @@
     </row>
     <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>75</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1304,7 +1304,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E1" s="13">
         <f>[2]STR_STAB!E$1</f>
@@ -1347,7 +1347,7 @@
     </row>
     <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>27</v>
@@ -1356,7 +1356,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" s="3">
         <v>0</v>
@@ -1364,7 +1364,7 @@
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>27</v>
@@ -1373,7 +1373,7 @@
         <v>25</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E5" s="24">
         <v>0</v>
@@ -1381,7 +1381,7 @@
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>27</v>
@@ -1390,7 +1390,7 @@
         <v>25</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
@@ -1398,7 +1398,7 @@
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>6</v>
@@ -1407,7 +1407,7 @@
         <v>26</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
@@ -1415,16 +1415,16 @@
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="20" t="s">
         <v>101</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>102</v>
       </c>
       <c r="E8" s="3">
         <v>0</v>
@@ -1441,7 +1441,7 @@
         <v>25</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E9" s="24">
         <v>0</v>
@@ -1449,33 +1449,33 @@
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="20" t="s">
         <v>72</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>73</v>
       </c>
       <c r="E11" s="24" t="s">
         <v>1</v>
@@ -1492,7 +1492,7 @@
         <v>26</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E12" s="3">
         <v>1</v>
@@ -1509,7 +1509,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
@@ -1571,7 +1571,7 @@
         <v>25</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
@@ -1579,19 +1579,19 @@
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>87</v>
-      </c>
       <c r="E18" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1605,7 +1605,7 @@
         <v>25</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E19" s="24">
         <v>0</v>
@@ -1613,19 +1613,19 @@
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>89</v>
-      </c>
       <c r="E20" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1639,7 +1639,7 @@
         <v>26</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E21" s="9">
         <v>0</v>
@@ -1656,7 +1656,7 @@
         <v>25</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
@@ -1664,19 +1664,19 @@
     </row>
     <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>92</v>
-      </c>
       <c r="E23" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1690,7 +1690,7 @@
         <v>26</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E24" s="25">
         <v>0</v>
@@ -1707,7 +1707,7 @@
         <v>26</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E25" s="25">
         <v>0</v>
@@ -1724,7 +1724,7 @@
         <v>26</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E26" s="25">
         <v>0</v>
@@ -1741,7 +1741,7 @@
         <v>26</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E27" s="25">
         <v>0</v>
@@ -1758,7 +1758,7 @@
         <v>26</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E28" s="25">
         <v>0</v>
@@ -1775,7 +1775,7 @@
         <v>26</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E29" s="25">
         <v>0</v>
@@ -1792,7 +1792,7 @@
         <v>25</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E30" s="3">
         <v>0</v>
@@ -1809,7 +1809,7 @@
         <v>26</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E31" s="3">
         <v>0</v>
@@ -1826,7 +1826,7 @@
         <v>26</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E32" s="3">
         <v>0</v>
@@ -1834,16 +1834,16 @@
     </row>
     <row r="33" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="20" t="s">
         <v>77</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>78</v>
       </c>
       <c r="E33" s="3" t="b">
         <v>0</v>
@@ -1860,7 +1860,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E1" s="13">
         <f>[2]STR_MIX!E$1</f>
@@ -1930,7 +1930,7 @@
     </row>
     <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>27</v>
@@ -1939,7 +1939,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" s="3">
         <v>0</v>
@@ -1947,24 +1947,24 @@
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>27</v>
@@ -1973,7 +1973,7 @@
         <v>25</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E6" s="24">
         <v>0</v>
@@ -1981,7 +1981,7 @@
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>27</v>
@@ -1990,7 +1990,7 @@
         <v>25</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
@@ -1998,7 +1998,7 @@
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>6</v>
@@ -2007,7 +2007,7 @@
         <v>26</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E8" s="3">
         <v>0</v>
@@ -2015,16 +2015,16 @@
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>101</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>102</v>
       </c>
       <c r="E9" s="3">
         <v>0</v>
@@ -2041,7 +2041,7 @@
         <v>25</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E10" s="24">
         <v>0</v>
@@ -2049,33 +2049,33 @@
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="20" t="s">
         <v>72</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>73</v>
       </c>
       <c r="E12" s="24" t="s">
         <v>1</v>
@@ -2092,7 +2092,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
@@ -2109,7 +2109,7 @@
         <v>26</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
@@ -2171,7 +2171,7 @@
         <v>25</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E18" s="3">
         <v>0</v>
@@ -2179,19 +2179,19 @@
     </row>
     <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>87</v>
-      </c>
       <c r="E19" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2205,7 +2205,7 @@
         <v>25</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E20" s="24">
         <v>0</v>
@@ -2213,19 +2213,19 @@
     </row>
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>89</v>
-      </c>
       <c r="E21" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2239,7 +2239,7 @@
         <v>26</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E22" s="9">
         <v>0</v>
@@ -2256,7 +2256,7 @@
         <v>25</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E23" s="3">
         <v>1</v>
@@ -2264,19 +2264,19 @@
     </row>
     <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>92</v>
-      </c>
       <c r="E24" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2290,7 +2290,7 @@
         <v>26</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E25" s="3">
         <v>1</v>
@@ -2307,7 +2307,7 @@
         <v>26</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E26" s="3">
         <v>3</v>
@@ -2324,7 +2324,7 @@
         <v>26</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E27" s="3">
         <v>250</v>
@@ -2341,7 +2341,7 @@
         <v>26</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E28" s="3">
         <v>10</v>
@@ -2358,7 +2358,7 @@
         <v>26</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E29" s="3">
         <v>20</v>
@@ -2375,7 +2375,7 @@
         <v>26</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E30" s="3">
         <v>0</v>
@@ -2392,7 +2392,7 @@
         <v>25</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E31" s="3">
         <v>0</v>
@@ -2409,7 +2409,7 @@
         <v>26</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E32" s="3">
         <v>0</v>
@@ -2426,7 +2426,7 @@
         <v>26</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E33" s="3">
         <v>0</v>
@@ -2434,16 +2434,16 @@
     </row>
     <row r="34" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="20" t="s">
         <v>77</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>78</v>
       </c>
       <c r="E34" s="3" t="b">
         <v>0</v>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E1" s="13">
         <f>[2]STR_SC!E$1</f>
@@ -2532,7 +2532,7 @@
     </row>
     <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>27</v>
@@ -2541,7 +2541,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" s="3">
         <v>0</v>
@@ -2549,24 +2549,24 @@
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>27</v>
@@ -2575,7 +2575,7 @@
         <v>25</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E6" s="24">
         <v>0</v>
@@ -2583,7 +2583,7 @@
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>27</v>
@@ -2592,7 +2592,7 @@
         <v>25</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
@@ -2600,7 +2600,7 @@
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>6</v>
@@ -2609,7 +2609,7 @@
         <v>26</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E8" s="3">
         <v>0</v>
@@ -2617,16 +2617,16 @@
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>101</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>102</v>
       </c>
       <c r="E9" s="3">
         <v>0</v>
@@ -2643,7 +2643,7 @@
         <v>25</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E10" s="24">
         <v>0</v>
@@ -2651,33 +2651,33 @@
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="20" t="s">
         <v>72</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>73</v>
       </c>
       <c r="E12" s="24" t="s">
         <v>1</v>
@@ -2694,7 +2694,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
@@ -2711,7 +2711,7 @@
         <v>26</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E14" s="3">
         <v>0</v>
@@ -2773,7 +2773,7 @@
         <v>25</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E18" s="3">
         <v>0</v>
@@ -2781,19 +2781,19 @@
     </row>
     <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>87</v>
-      </c>
       <c r="E19" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2807,7 +2807,7 @@
         <v>25</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E20" s="3">
         <v>0</v>
@@ -2815,19 +2815,19 @@
     </row>
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>92</v>
-      </c>
       <c r="E21" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2841,7 +2841,7 @@
         <v>26</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E22" s="8">
         <v>0</v>
@@ -2858,7 +2858,7 @@
         <v>26</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E23" s="8">
         <v>0</v>
@@ -2875,7 +2875,7 @@
         <v>26</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E24" s="8">
         <v>0</v>
@@ -2892,7 +2892,7 @@
         <v>26</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E25" s="25">
         <v>0</v>
@@ -2909,7 +2909,7 @@
         <v>26</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E26" s="25">
         <v>0</v>
@@ -2926,7 +2926,7 @@
         <v>26</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27" s="25">
         <v>0</v>
@@ -2943,7 +2943,7 @@
         <v>25</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E28" s="25">
         <v>0</v>
@@ -2960,7 +2960,7 @@
         <v>26</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E29" s="25">
         <v>0</v>
@@ -2977,7 +2977,7 @@
         <v>26</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E30" s="25">
         <v>0</v>
@@ -2994,7 +2994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D22" sqref="D22"/>
       <selection pane="topRight" activeCell="D22" sqref="D22"/>
@@ -3023,7 +3023,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E1" s="13">
         <f>[2]Z_JACKET!E$1</f>
@@ -3066,7 +3066,7 @@
     </row>
     <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>27</v>
@@ -3075,7 +3075,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" s="3">
         <v>0</v>
@@ -3083,19 +3083,19 @@
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3109,7 +3109,7 @@
         <v>25</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E6" s="24">
         <v>0</v>
@@ -3117,33 +3117,33 @@
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="20" t="s">
         <v>72</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>73</v>
       </c>
       <c r="E8" s="24" t="s">
         <v>1</v>
@@ -3160,7 +3160,7 @@
         <v>26</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E9" s="3">
         <v>0</v>
@@ -3177,7 +3177,7 @@
         <v>26</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E10" s="3">
         <v>0</v>
@@ -3239,7 +3239,7 @@
         <v>25</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" s="3">
         <v>0</v>
@@ -3247,19 +3247,19 @@
     </row>
     <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>87</v>
-      </c>
       <c r="E15" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3273,7 +3273,7 @@
         <v>25</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
@@ -3281,19 +3281,19 @@
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>92</v>
-      </c>
       <c r="E17" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3307,7 +3307,7 @@
         <v>26</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E18" s="3">
         <v>0</v>
@@ -3324,7 +3324,7 @@
         <v>26</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" s="3">
         <v>0</v>
@@ -3341,7 +3341,7 @@
         <v>26</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E20" s="3">
         <v>0</v>
@@ -3358,7 +3358,7 @@
         <v>26</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E21" s="3">
         <v>0</v>
@@ -3375,7 +3375,7 @@
         <v>26</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
@@ -3392,7 +3392,7 @@
         <v>25</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E23" s="3">
         <v>0</v>
@@ -3409,7 +3409,7 @@
         <v>26</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E24" s="3">
         <v>0</v>
@@ -3426,7 +3426,7 @@
         <v>26</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E25" s="3">
         <v>0</v>

</xml_diff>

<commit_message>
chore: add flag IOP_INTERPOLATION
Addedd flag IOP_INTERPOLATION in sheet STACK of input tile template_conductor_1_operation.xlsx

modified:   input_files/input_file_template/template_conductor_1_operation.xlsx
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_1_operation.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_1_operation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3EFA9B-407E-4A05-A0CC-8AD9A4A1EEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14622D91-E11C-4657-922E-373A51A113C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4845" yWindow="3855" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAN" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="111">
   <si>
     <t>IBIFUN</t>
   </si>
@@ -981,7 +981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -1273,14 +1273,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04312A78-FBC2-476F-A763-194D3CD2A19F}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D10" sqref="D10"/>
       <selection pane="topRight" activeCell="D10" sqref="D10"/>
       <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,51 +1363,51 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D6" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="B7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D7" s="20" t="s">
         <v>96</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>98</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
@@ -1415,58 +1415,58 @@
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B9" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="20" t="s">
+      <c r="C9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D10" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="E10" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>82</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>70</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>27</v>
@@ -1475,32 +1475,32 @@
         <v>71</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>1</v>
+        <v>79</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E12" s="3">
+        <v>72</v>
+      </c>
+      <c r="E12" s="24" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>1</v>
@@ -1509,30 +1509,32 @@
         <v>26</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="23" t="s">
+      <c r="A14" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="23">
-        <v>0</v>
+      <c r="C14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="23" t="s">
         <v>1</v>
@@ -1547,10 +1549,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>26</v>
@@ -1560,145 +1562,143 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D18" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="B19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D19" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="B20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D20" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="E20" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="B21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D21" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="20" t="s">
+      <c r="B22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="E22" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="B23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D23" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="B24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D24" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="25">
-        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>6</v>
@@ -1707,7 +1707,7 @@
         <v>26</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E25" s="25">
         <v>0</v>
@@ -1715,16 +1715,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E26" s="25">
         <v>0</v>
@@ -1732,16 +1732,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E27" s="25">
         <v>0</v>
@@ -1749,7 +1749,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>8</v>
@@ -1758,58 +1758,58 @@
         <v>26</v>
       </c>
       <c r="D28" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
+      <c r="E29" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="20" t="s">
+      <c r="B30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E29" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+      <c r="E30" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="B31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D31" s="20" t="s">
         <v>102</v>
-      </c>
-      <c r="E30" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>103</v>
       </c>
       <c r="E31" s="3">
         <v>0</v>
@@ -1817,7 +1817,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>14</v>
@@ -1826,26 +1826,43 @@
         <v>26</v>
       </c>
       <c r="D32" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="E32" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="B34" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D33" s="20" t="s">
+      <c r="D34" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="E33" s="3" t="b">
+      <c r="E34" s="3" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1860,10 +1877,10 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2465,7 +2482,7 @@
       <selection activeCell="D22" sqref="D22"/>
       <selection pane="topRight" activeCell="D22" sqref="D22"/>
       <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2994,12 +3011,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D22" sqref="D22"/>
       <selection pane="topRight" activeCell="D22" sqref="D22"/>
       <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
-      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
doc: update documentation in file template_conductor_1_operation
Added comment related to the necessity of specify the value of TQBEG in the input file also if the heating is read from intput file since it will somehow influence the evaluation of the heat transfer coefficient between fluid and solid component if there is an interface and if it is evaluated by the software. A better solution should be found but for the time being it is a good quick fix.

modified:   input_files/input_file_template/template_conductor_1_operation.xlsx
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_1_operation.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_1_operation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele.Placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14622D91-E11C-4657-922E-373A51A113C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC995AB-268A-4F58-A795-9A3F7BA553DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4845" yWindow="3855" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAN" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="113">
   <si>
     <t>IBIFUN</t>
   </si>
@@ -184,9 +184,6 @@
     <t>power density in each strand</t>
   </si>
   <si>
-    <t>heating start time</t>
-  </si>
-  <si>
     <t>heating end time</t>
   </si>
   <si>
@@ -374,6 +371,38 @@
   </si>
   <si>
     <t>flag to define initialization and the hydraulic boundary conditions (&gt;0 value from below, &lt;0 valure from input file: press.dat, temp.dat, mdot.dat). 1 = inlet and outlet pressure, inlet (outlet) temperaure; 2 = inlet pressure and temperature, outlet mass flow rate; 3 = inlet mass flow rate and temperature, outlet pressure.</t>
+  </si>
+  <si>
+    <t>heating end time.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">heating start time. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Recommended</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: add the time at with the heating starts also if the heat is from external file, IQFUN = -1 (requested for the correct evaluation of htc between fluid and solid)</t>
+    </r>
+  </si>
+  <si>
+    <t>heating start time. Recommended: add the time at with the heating starts also if the heat is from external file, IQFUN = -1 (requested for the correct evaluation of htc between fluid and solid)</t>
   </si>
 </sst>
 </file>
@@ -562,7 +591,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="CHAN"/>
@@ -629,7 +658,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="CHAN"/>
@@ -988,17 +1017,17 @@
       <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.140625" style="4" customWidth="1"/>
-    <col min="5" max="6" width="17.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="5"/>
+    <col min="1" max="1" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.1796875" style="4" customWidth="1"/>
+    <col min="5" max="6" width="17.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="str">
         <f>[1]CHAN!$A$1</f>
         <v>CHAN</v>
@@ -1020,7 +1049,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="6"/>
@@ -1036,7 +1065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="str">
         <f>[1]CHAN!A$3</f>
         <v>Variable name</v>
@@ -1062,7 +1091,7 @@
         <v>CHAN_2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
         <v>9</v>
       </c>
@@ -1073,7 +1102,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E4" s="3">
         <v>2</v>
@@ -1082,7 +1111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1093,7 +1122,7 @@
         <v>26</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" s="3">
         <v>4.5</v>
@@ -1102,7 +1131,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -1113,7 +1142,7 @@
         <v>26</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" s="3">
         <v>4.5</v>
@@ -1122,7 +1151,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -1133,7 +1162,7 @@
         <v>26</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" s="3">
         <v>4.5</v>
@@ -1142,7 +1171,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -1153,7 +1182,7 @@
         <v>26</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" s="9">
         <v>600000</v>
@@ -1162,7 +1191,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -1173,7 +1202,7 @@
         <v>26</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="9">
         <v>590000</v>
@@ -1182,7 +1211,7 @@
         <v>590000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -1193,7 +1222,7 @@
         <v>26</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" s="9">
         <f>600000</f>
@@ -1204,7 +1233,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
@@ -1215,7 +1244,7 @@
         <v>26</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="3">
         <v>8.3999999999999995E-3</v>
@@ -1224,9 +1253,9 @@
         <v>1.248E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>17</v>
@@ -1235,7 +1264,7 @@
         <v>26</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E12" s="3">
         <v>0</v>
@@ -1244,24 +1273,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>74</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1275,25 +1304,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04312A78-FBC2-476F-A763-194D3CD2A19F}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D10" sqref="D10"/>
       <selection pane="topRight" activeCell="D10" sqref="D10"/>
       <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:E34"/>
+      <selection pane="bottomRight" activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.42578125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="5"/>
+    <col min="1" max="1" width="27.7265625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.453125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="str">
         <f>[1]STACK!$A$1</f>
         <v>STACK</v>
@@ -1304,14 +1333,14 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E1" s="13">
         <f>[2]STR_STAB!E$1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="18"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1323,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -1345,9 +1374,9 @@
         <v>STACK_0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>27</v>
@@ -1356,32 +1385,32 @@
         <v>25</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E4" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>27</v>
@@ -1390,15 +1419,15 @@
         <v>25</v>
       </c>
       <c r="D6" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="27" t="s">
         <v>94</v>
-      </c>
-      <c r="E6" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
-        <v>95</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>27</v>
@@ -1407,15 +1436,15 @@
         <v>25</v>
       </c>
       <c r="D7" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="27" t="s">
         <v>96</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
-        <v>97</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>6</v>
@@ -1424,30 +1453,30 @@
         <v>26</v>
       </c>
       <c r="D8" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="B9" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>101</v>
-      </c>
       <c r="E9" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
         <v>0</v>
       </c>
@@ -1458,47 +1487,47 @@
         <v>25</v>
       </c>
       <c r="D10" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>82</v>
-      </c>
       <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="20" t="s">
         <v>71</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>72</v>
       </c>
       <c r="E12" s="24" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>19</v>
       </c>
@@ -1509,13 +1538,13 @@
         <v>26</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>20</v>
       </c>
@@ -1526,13 +1555,13 @@
         <v>26</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>21</v>
       </c>
@@ -1547,7 +1576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>22</v>
       </c>
@@ -1562,7 +1591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>23</v>
       </c>
@@ -1577,7 +1606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
         <v>2</v>
       </c>
@@ -1594,24 +1623,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>86</v>
-      </c>
       <c r="E19" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
         <v>3</v>
       </c>
@@ -1628,24 +1657,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>88</v>
-      </c>
       <c r="E21" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
         <v>4</v>
       </c>
@@ -1662,7 +1691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
         <v>34</v>
       </c>
@@ -1673,30 +1702,30 @@
         <v>25</v>
       </c>
       <c r="D23" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+      <c r="B24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>91</v>
-      </c>
       <c r="E24" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>35</v>
       </c>
@@ -1713,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
         <v>36</v>
       </c>
@@ -1730,7 +1759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
         <v>5</v>
       </c>
@@ -1747,7 +1776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
         <v>37</v>
       </c>
@@ -1758,13 +1787,13 @@
         <v>26</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="E28" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="15" t="s">
         <v>38</v>
       </c>
@@ -1775,13 +1804,13 @@
         <v>26</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
       <c r="E29" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
         <v>24</v>
       </c>
@@ -1792,13 +1821,13 @@
         <v>26</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E30" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
         <v>9</v>
       </c>
@@ -1809,13 +1838,13 @@
         <v>25</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E31" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
         <v>10</v>
       </c>
@@ -1826,13 +1855,13 @@
         <v>26</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E32" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
         <v>11</v>
       </c>
@@ -1843,24 +1872,24 @@
         <v>26</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E33" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A34" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="20" t="s">
         <v>76</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>77</v>
       </c>
       <c r="E34" s="3" t="b">
         <v>0</v>
@@ -1877,23 +1906,23 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:E34"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.42578125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="5"/>
+    <col min="1" max="1" width="27.7265625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.453125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="str">
         <f>[1]STR_MIX!$A$1</f>
         <v>STR_MIX</v>
@@ -1911,7 +1940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="18"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1923,7 +1952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -1945,9 +1974,9 @@
         <v>STR_MIX_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>27</v>
@@ -1956,32 +1985,32 @@
         <v>25</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E4" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>27</v>
@@ -1990,15 +2019,15 @@
         <v>25</v>
       </c>
       <c r="D6" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="27" t="s">
         <v>94</v>
-      </c>
-      <c r="E6" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
-        <v>95</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>27</v>
@@ -2007,15 +2036,15 @@
         <v>25</v>
       </c>
       <c r="D7" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="27" t="s">
         <v>96</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
-        <v>97</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>6</v>
@@ -2024,30 +2053,30 @@
         <v>26</v>
       </c>
       <c r="D8" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="B9" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>101</v>
-      </c>
       <c r="E9" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
         <v>0</v>
       </c>
@@ -2058,47 +2087,47 @@
         <v>25</v>
       </c>
       <c r="D10" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>82</v>
-      </c>
       <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="20" t="s">
         <v>71</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>72</v>
       </c>
       <c r="E12" s="24" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>19</v>
       </c>
@@ -2109,13 +2138,13 @@
         <v>26</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>20</v>
       </c>
@@ -2126,13 +2155,13 @@
         <v>26</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>21</v>
       </c>
@@ -2147,7 +2176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>22</v>
       </c>
@@ -2162,7 +2191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>23</v>
       </c>
@@ -2177,7 +2206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
         <v>2</v>
       </c>
@@ -2194,24 +2223,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>86</v>
-      </c>
       <c r="E19" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
         <v>3</v>
       </c>
@@ -2228,24 +2257,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>88</v>
-      </c>
       <c r="E21" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
         <v>4</v>
       </c>
@@ -2262,7 +2291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
         <v>34</v>
       </c>
@@ -2273,30 +2302,30 @@
         <v>25</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E23" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>91</v>
-      </c>
       <c r="E24" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>35</v>
       </c>
@@ -2313,7 +2342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
         <v>36</v>
       </c>
@@ -2330,7 +2359,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
         <v>5</v>
       </c>
@@ -2347,7 +2376,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
         <v>37</v>
       </c>
@@ -2358,13 +2387,13 @@
         <v>26</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="E28" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="15" t="s">
         <v>38</v>
       </c>
@@ -2375,13 +2404,13 @@
         <v>26</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E29" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
         <v>24</v>
       </c>
@@ -2392,13 +2421,13 @@
         <v>26</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E30" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
         <v>9</v>
       </c>
@@ -2409,13 +2438,13 @@
         <v>25</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E31" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
         <v>10</v>
       </c>
@@ -2426,13 +2455,13 @@
         <v>26</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E32" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
         <v>11</v>
       </c>
@@ -2443,24 +2472,24 @@
         <v>26</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E33" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A34" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="20" t="s">
         <v>76</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>77</v>
       </c>
       <c r="E34" s="3" t="b">
         <v>0</v>
@@ -2478,24 +2507,24 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D22" sqref="D22"/>
       <selection pane="topRight" activeCell="D22" sqref="D22"/>
       <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4:E27"/>
+      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="5"/>
+    <col min="1" max="1" width="27.7265625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.453125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="str">
         <f>[1]STR_STAB!$A$1</f>
         <v>STR_STAB</v>
@@ -2506,14 +2535,14 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E1" s="13">
         <f>[2]STR_SC!E$1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="18"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2525,7 +2554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -2547,9 +2576,9 @@
         <v>STR_STAB_0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>27</v>
@@ -2558,32 +2587,32 @@
         <v>25</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E4" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>27</v>
@@ -2592,15 +2621,15 @@
         <v>25</v>
       </c>
       <c r="D6" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="27" t="s">
         <v>94</v>
-      </c>
-      <c r="E6" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
-        <v>95</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>27</v>
@@ -2609,15 +2638,15 @@
         <v>25</v>
       </c>
       <c r="D7" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="27" t="s">
         <v>96</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
-        <v>97</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>6</v>
@@ -2626,30 +2655,30 @@
         <v>26</v>
       </c>
       <c r="D8" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="B9" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>101</v>
-      </c>
       <c r="E9" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
         <v>0</v>
       </c>
@@ -2660,47 +2689,47 @@
         <v>25</v>
       </c>
       <c r="D10" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>82</v>
-      </c>
       <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="20" t="s">
         <v>71</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>72</v>
       </c>
       <c r="E12" s="24" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>19</v>
       </c>
@@ -2711,13 +2740,13 @@
         <v>26</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>20</v>
       </c>
@@ -2728,13 +2757,13 @@
         <v>26</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E14" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>21</v>
       </c>
@@ -2749,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>22</v>
       </c>
@@ -2764,7 +2793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>23</v>
       </c>
@@ -2779,7 +2808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
         <v>2</v>
       </c>
@@ -2796,24 +2825,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>86</v>
-      </c>
       <c r="E19" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
         <v>34</v>
       </c>
@@ -2824,30 +2853,30 @@
         <v>25</v>
       </c>
       <c r="D20" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="B21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>91</v>
-      </c>
       <c r="E21" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
         <v>35</v>
       </c>
@@ -2864,7 +2893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
         <v>36</v>
       </c>
@@ -2881,7 +2910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
         <v>5</v>
       </c>
@@ -2898,7 +2927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>37</v>
       </c>
@@ -2908,14 +2937,14 @@
       <c r="C25" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>47</v>
+      <c r="D25" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="E25" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
         <v>38</v>
       </c>
@@ -2926,13 +2955,13 @@
         <v>26</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
         <v>24</v>
       </c>
@@ -2943,13 +2972,13 @@
         <v>26</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
         <v>9</v>
       </c>
@@ -2960,13 +2989,13 @@
         <v>25</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E28" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="15" t="s">
         <v>10</v>
       </c>
@@ -2977,13 +3006,13 @@
         <v>26</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E29" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
         <v>11</v>
       </c>
@@ -2994,7 +3023,7 @@
         <v>26</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E30" s="25">
         <v>0</v>
@@ -3011,25 +3040,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D22" sqref="D22"/>
       <selection pane="topRight" activeCell="D22" sqref="D22"/>
       <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4:E22"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="5"/>
+    <col min="1" max="1" width="14.453125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.453125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="str">
         <f>[1]Z_JACKET!$A$1</f>
         <v>Z_JACKET</v>
@@ -3040,14 +3069,14 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E1" s="13">
         <f>[2]Z_JACKET!E$1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="18"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3059,7 +3088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -3081,9 +3110,9 @@
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>27</v>
@@ -3092,30 +3121,30 @@
         <v>25</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E4" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
         <v>0</v>
       </c>
@@ -3126,47 +3155,47 @@
         <v>25</v>
       </c>
       <c r="D6" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E6" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>82</v>
-      </c>
       <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="20" t="s">
         <v>71</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>72</v>
       </c>
       <c r="E8" s="24" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>19</v>
       </c>
@@ -3177,13 +3206,13 @@
         <v>26</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E9" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
         <v>20</v>
       </c>
@@ -3194,13 +3223,13 @@
         <v>26</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E10" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
         <v>21</v>
       </c>
@@ -3215,7 +3244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>22</v>
       </c>
@@ -3230,7 +3259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="19" t="s">
         <v>23</v>
       </c>
@@ -3245,7 +3274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>2</v>
       </c>
@@ -3262,24 +3291,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>86</v>
-      </c>
       <c r="E15" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
         <v>34</v>
       </c>
@@ -3290,30 +3319,30 @@
         <v>25</v>
       </c>
       <c r="D16" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E16" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="B17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>91</v>
-      </c>
       <c r="E17" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
         <v>35</v>
       </c>
@@ -3330,7 +3359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
         <v>36</v>
       </c>
@@ -3347,7 +3376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
         <v>5</v>
       </c>
@@ -3358,13 +3387,13 @@
         <v>26</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E20" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
         <v>37</v>
       </c>
@@ -3374,14 +3403,14 @@
       <c r="C21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>47</v>
+      <c r="D21" s="20" t="s">
+        <v>111</v>
       </c>
       <c r="E21" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
         <v>38</v>
       </c>
@@ -3392,13 +3421,13 @@
         <v>26</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
         <v>9</v>
       </c>
@@ -3409,13 +3438,13 @@
         <v>25</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E23" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
         <v>10</v>
       </c>
@@ -3426,13 +3455,13 @@
         <v>26</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E24" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>11</v>
       </c>
@@ -3443,7 +3472,7 @@
         <v>26</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E25" s="3">
         <v>0</v>

</xml_diff>